<commit_message>
update timecard and added install.sh
</commit_message>
<xml_diff>
--- a/docs/school/WorkLog-PiersenSchuiling.xlsx
+++ b/docs/school/WorkLog-PiersenSchuiling.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t xml:space="preserve">Work Log for Computer Applications Practicum</t>
   </si>
@@ -203,6 +203,21 @@
   </si>
   <si>
     <t xml:space="preserve">Adding list of edges to road segments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finding seg fault in Test::followPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuring project for Windows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correcting incident edges to detect proper edge and road segment in Test::followPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finishing final tests and filling out Test Results Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finishing Testing Document, User Documentation, and remaining final submissions</t>
   </si>
 </sst>
 </file>
@@ -568,11 +583,11 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N66" activeCellId="0" sqref="N66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
@@ -614,7 +629,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
@@ -639,7 +654,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
         <v>45555</v>
       </c>
@@ -662,7 +677,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
         <v>45556</v>
       </c>
@@ -685,7 +700,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <v>45561</v>
       </c>
@@ -702,7 +717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
         <v>45562</v>
       </c>
@@ -736,7 +751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>45539</v>
       </c>
@@ -753,7 +768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
         <v>45541</v>
       </c>
@@ -770,7 +785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="n">
         <v>45542</v>
       </c>
@@ -787,7 +802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="n">
         <v>45544</v>
       </c>
@@ -804,7 +819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="n">
         <v>45555</v>
       </c>
@@ -821,7 +836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="n">
         <v>45556</v>
       </c>
@@ -838,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="n">
         <v>45561</v>
       </c>
@@ -855,7 +870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>45562</v>
       </c>
@@ -872,7 +887,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="n">
         <v>45566</v>
       </c>
@@ -889,7 +904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="n">
         <v>45573</v>
       </c>
@@ -906,7 +921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
         <v>45576</v>
       </c>
@@ -1689,22 +1704,106 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="13"/>
+      <c r="A68" s="13" t="n">
+        <v>45769</v>
+      </c>
+      <c r="B68" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="C68" s="17" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13"/>
+      <c r="A69" s="13" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B69" s="17" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C69" s="17" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="13"/>
+      <c r="A70" s="13" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B70" s="17" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="C70" s="17" t="n">
+        <v>0.822916666666667</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="13"/>
+      <c r="A71" s="13" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B71" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="C71" s="17" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="13"/>
+      <c r="A72" s="13" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B72" s="17" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C72" s="17" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="13"/>
+      <c r="A73" s="13" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B73" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="C73" s="17" t="n">
+        <v>0.979166666666667</v>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="13"/>

</xml_diff>